<commit_message>
Added data to sample csv test
</commit_message>
<xml_diff>
--- a/Weka/Sample CSV Test.xlsx
+++ b/Weka/Sample CSV Test.xlsx
@@ -24,12 +24,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Outlook</t>
   </si>
   <si>
     <t>Temperature</t>
+  </si>
+  <si>
+    <t>Humidity</t>
+  </si>
+  <si>
+    <t>Windy</t>
+  </si>
+  <si>
+    <t>Play</t>
   </si>
 </sst>
 </file>
@@ -381,21 +390,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>